<commit_message>
fix plots and add some new data
</commit_message>
<xml_diff>
--- a/010_data/2020_CT.xlsx
+++ b/010_data/2020_CT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Box/Documents/Hanks-Research/2020_Kestrel_Plots/010_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/Hanks-Research/2020_Kestrel_Plots/010_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{153E0099-698F-F248-BAE5-79ADC71A8BF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D68177A-2577-4B46-8B62-D6149C36B0D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1820" yWindow="1460" windowWidth="26600" windowHeight="16040" xr2:uid="{44307CE2-7908-8D46-B53C-9D283CE81B44}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>total # of chicks</t>
   </si>
@@ -102,13 +102,22 @@
   </si>
   <si>
     <t>           4.1</t>
+  </si>
+  <si>
+    <t>org</t>
+  </si>
+  <si>
+    <t>Gingert &amp; Dudek</t>
+  </si>
+  <si>
+    <t>Sayers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,6 +128,12 @@
     <font>
       <sz val="15"/>
       <color rgb="FF1A1A1A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -143,9 +158,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,148 +476,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54ABF50-F9D9-314C-AC71-9E664F690E33}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="31.6640625" customWidth="1"/>
-    <col min="3" max="3" width="44.5" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="4" max="4" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1">
         <v>2010</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1">
         <v>2011</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1">
         <v>2012</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1">
         <v>2013</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1">
         <v>2014</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1">
         <v>2015</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+    <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1">
         <v>2016</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+    <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1">
         <v>2017</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+    <row r="10" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1">
         <v>2018</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+    <row r="11" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1">
         <v>2019</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+    <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1">
         <v>2020</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2018</v>
+      </c>
+      <c r="C13">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C14">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C15">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>